<commit_message>
fix read para_list bugs
</commit_message>
<xml_diff>
--- a/Library/DPU01_Lib Demo3.xlsx
+++ b/Library/DPU01_Lib Demo3.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Info" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>DPU01_Lib Demo3</t>
   </si>
@@ -141,6 +142,18 @@
   </si>
   <si>
     <t>HTR HL Alarm</t>
+  </si>
+  <si>
+    <t>Page count</t>
+  </si>
+  <si>
+    <t>Page list</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -776,4 +789,42 @@
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>